<commit_message>
first 6 crop graphs added
</commit_message>
<xml_diff>
--- a/Elixir Crop & Soil Information/SoilTables.xlsx
+++ b/Elixir Crop & Soil Information/SoilTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CTIS\Year_4\Sem_2\CTIS - Senior 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berkozdoruk/Desktop/GitHub/Elixir-Documentation/Elixir Crop &amp; Soil Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD218DA7-9B80-466C-93DA-0336FBC36B84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC06AC64-E78B-1E44-AFD2-3EFCCD6A66FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9426C972-A351-456A-ACBE-3D80CCCA88B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9426C972-A351-456A-ACBE-3D80CCCA88B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Tables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="29">
   <si>
     <t>Sand</t>
   </si>
@@ -76,24 +76,6 @@
     <t>http://soilquality.org.au/factsheets/water-availability</t>
   </si>
   <si>
-    <t>Table 1</t>
-  </si>
-  <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Table 4</t>
-  </si>
-  <si>
-    <t>Table 5</t>
-  </si>
-  <si>
-    <t>Table 6</t>
-  </si>
-  <si>
     <t>Table 7</t>
   </si>
   <si>
@@ -104,6 +86,33 @@
   </si>
   <si>
     <t>Table 10</t>
+  </si>
+  <si>
+    <t>domates</t>
+  </si>
+  <si>
+    <t>clay</t>
+  </si>
+  <si>
+    <t>clay loam</t>
+  </si>
+  <si>
+    <t>Domates</t>
+  </si>
+  <si>
+    <t>Salatalik</t>
+  </si>
+  <si>
+    <t>Ankara Armudu</t>
+  </si>
+  <si>
+    <t>Elma</t>
+  </si>
+  <si>
+    <t>Biber</t>
+  </si>
+  <si>
+    <t>Marul</t>
   </si>
 </sst>
 </file>
@@ -156,18 +165,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -186,7 +197,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1026,7 +1037,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1674,7 +1685,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2322,7 +2333,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2340,7 +2351,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 2</c:v>
+              <c:v>Salatalik</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -2590,22 +2601,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2672,22 +2683,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2970,7 +2981,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2988,7 +2999,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 1</c:v>
+              <c:v>Domates</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -3238,22 +3249,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3320,22 +3331,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3518,6 +3529,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1891941872"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3609,7 +3621,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3627,7 +3639,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 3</c:v>
+              <c:v>Ankara Armudu</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -3877,22 +3889,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="d\-mmm">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3959,22 +3971,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4257,7 +4269,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4275,7 +4287,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 4</c:v>
+              <c:v>Elma</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -4525,22 +4537,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4607,22 +4619,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4905,7 +4917,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4923,7 +4935,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 5</c:v>
+              <c:v>Biber</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -5173,22 +5185,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5255,22 +5267,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5553,7 +5565,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5571,7 +5583,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 6</c:v>
+              <c:v>Marul</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -5821,22 +5833,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5903,22 +5915,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6201,7 +6213,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6849,7 +6861,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -14160,11 +14172,72 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>319776</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Resim 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B1410B-824A-B249-BFED-288F650F51F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17316824" y="6604000"/>
+          <a:ext cx="5698599" cy="4900706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -14460,25 +14533,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD730A-B317-4AF4-A2AA-E14D92B6C330}">
-  <dimension ref="C2:AA206"/>
+  <dimension ref="C2:AB206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC34" sqref="AC34"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H156" sqref="H156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="3" t="s">
+    <row r="2" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="5"/>
     </row>
-    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>6</v>
       </c>
@@ -14501,7 +14574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>14</v>
       </c>
@@ -14524,7 +14597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
@@ -14547,7 +14620,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>14</v>
       </c>
@@ -14570,7 +14643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
@@ -14593,13 +14666,13 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="28" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="E28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="4"/>
+    <row r="28" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="E28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>6</v>
       </c>
@@ -14622,33 +14695,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G30" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H30" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I30" s="1">
+        <v>19</v>
+      </c>
+      <c r="J30" s="1">
         <v>24</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <v>28</v>
       </c>
-      <c r="K30" s="1">
-        <v>80</v>
-      </c>
-      <c r="AA30" s="5" t="s">
+      <c r="AA30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C31" s="2"/>
       <c r="E31" s="2" t="s">
         <v>12</v>
@@ -14664,31 +14737,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C32" s="2"/>
       <c r="E32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G32" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H32" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I32" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J32" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K32" s="1">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="33" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E33" s="2" t="s">
         <v>13</v>
       </c>
@@ -14703,16 +14776,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="F44" s="4"/>
+    <row r="44" spans="5:23" x14ac:dyDescent="0.2">
+      <c r="F44" s="3"/>
     </row>
-    <row r="46" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E46" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F46" s="4"/>
+    <row r="46" spans="5:23" x14ac:dyDescent="0.2">
+      <c r="E46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>6</v>
       </c>
@@ -14735,32 +14808,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G48" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H48" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I48" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J48" s="1">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K48" s="1">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
     </row>
-    <row r="49" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E49" s="2" t="s">
         <v>12</v>
       </c>
@@ -14779,30 +14852,30 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F50" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H50" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I50" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J50" s="1">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="K50" s="1">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="51" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E51" s="2" t="s">
         <v>13</v>
       </c>
@@ -14821,13 +14894,51 @@
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="4"/>
+    <row r="62" spans="5:28" x14ac:dyDescent="0.2">
+      <c r="Y62" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z62">
+        <v>60</v>
+      </c>
+      <c r="AB62">
+        <v>80</v>
+      </c>
     </row>
-    <row r="68" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:28" x14ac:dyDescent="0.2">
+      <c r="Y64" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z64" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB64" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="65" spans="5:28" x14ac:dyDescent="0.2">
+      <c r="Z65" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="AB65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="5:28" x14ac:dyDescent="0.2">
+      <c r="Z66">
+        <v>60</v>
+      </c>
+      <c r="AB66">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="5:28" x14ac:dyDescent="0.2">
+      <c r="E67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
         <v>6</v>
       </c>
@@ -14849,31 +14960,34 @@
       <c r="K68" t="s">
         <v>5</v>
       </c>
+      <c r="Y68" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="69" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F69" s="1">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="G69" s="1">
-        <v>12</v>
-      </c>
-      <c r="H69" s="1">
-        <v>18</v>
+        <v>0.5</v>
+      </c>
+      <c r="H69" s="7">
+        <v>2</v>
       </c>
       <c r="I69" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="J69" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="K69" s="1">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="70" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E70" s="2" t="s">
         <v>12</v>
       </c>
@@ -14888,30 +15002,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F71" s="1">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="G71" s="1">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="H71" s="1">
-        <v>5</v>
+        <v>1.3</v>
       </c>
       <c r="I71" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J71" s="1">
-        <v>11</v>
+        <v>5.2</v>
       </c>
       <c r="K71" s="1">
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E72" s="2" t="s">
         <v>13</v>
       </c>
@@ -14926,7 +15040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -14935,7 +15049,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -14944,7 +15058,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="88" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -14953,13 +15067,13 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" s="4"/>
+    <row r="89" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E90" t="s">
         <v>6</v>
       </c>
@@ -14982,30 +15096,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E91" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F91" s="1">
+        <v>3</v>
+      </c>
+      <c r="G91" s="1">
         <v>5</v>
       </c>
-      <c r="G91" s="1">
+      <c r="H91" s="1">
+        <v>6</v>
+      </c>
+      <c r="I91" s="1">
+        <v>8</v>
+      </c>
+      <c r="J91" s="1">
+        <v>10</v>
+      </c>
+      <c r="K91" s="1">
         <v>12</v>
       </c>
-      <c r="H91" s="1">
-        <v>18</v>
-      </c>
-      <c r="I91" s="1">
-        <v>24</v>
-      </c>
-      <c r="J91" s="1">
-        <v>28</v>
-      </c>
-      <c r="K91" s="1">
-        <v>60</v>
-      </c>
     </row>
-    <row r="92" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E92" s="2" t="s">
         <v>12</v>
       </c>
@@ -15020,30 +15134,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F93" s="1">
+        <v>2</v>
+      </c>
+      <c r="G93" s="1">
         <v>3</v>
       </c>
-      <c r="G93" s="1">
+      <c r="H93" s="1">
         <v>4</v>
       </c>
-      <c r="H93" s="1">
+      <c r="I93" s="1">
         <v>5</v>
       </c>
-      <c r="I93" s="1">
-        <v>10</v>
-      </c>
       <c r="J93" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K93" s="1">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="94" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E94" s="2" t="s">
         <v>13</v>
       </c>
@@ -15058,13 +15172,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E107" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F107" s="4"/>
+    <row r="107" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E107" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E108" t="s">
         <v>6</v>
       </c>
@@ -15087,30 +15201,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E109" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G109" s="1">
+        <v>9</v>
+      </c>
+      <c r="H109" s="1">
         <v>12</v>
       </c>
-      <c r="H109" s="1">
-        <v>18</v>
-      </c>
       <c r="I109" s="1">
+        <v>16</v>
+      </c>
+      <c r="J109" s="1">
+        <v>20</v>
+      </c>
+      <c r="K109" s="1">
         <v>24</v>
       </c>
-      <c r="J109" s="1">
-        <v>28</v>
-      </c>
-      <c r="K109" s="1">
-        <v>50</v>
-      </c>
     </row>
-    <row r="110" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E110" s="2" t="s">
         <v>12</v>
       </c>
@@ -15125,30 +15239,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E111" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F111" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G111" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H111" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I111" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J111" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K111" s="1">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="112" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E112" s="2" t="s">
         <v>13</v>
       </c>
@@ -15163,13 +15277,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E127" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F127" s="4"/>
+    <row r="127" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E127" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E128" t="s">
         <v>6</v>
       </c>
@@ -15192,30 +15306,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E129" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F129" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G129" s="1">
         <v>12</v>
       </c>
       <c r="H129" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I129" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J129" s="1">
         <v>28</v>
       </c>
       <c r="K129" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="130" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E130" s="2" t="s">
         <v>12</v>
       </c>
@@ -15230,30 +15344,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E131" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F131" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G131" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H131" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I131" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J131" s="1">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K131" s="1">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="132" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E132" s="2" t="s">
         <v>13</v>
       </c>
@@ -15268,13 +15382,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E147" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F147" s="4"/>
+    <row r="147" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E147" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F147" s="3"/>
     </row>
-    <row r="148" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E148" t="s">
         <v>6</v>
       </c>
@@ -15297,7 +15411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E149" s="1" t="s">
         <v>10</v>
       </c>
@@ -15320,7 +15434,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="150" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E150" s="2" t="s">
         <v>12</v>
       </c>
@@ -15335,7 +15449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E151" s="1" t="s">
         <v>11</v>
       </c>
@@ -15358,7 +15472,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E152" s="2" t="s">
         <v>13</v>
       </c>
@@ -15373,13 +15487,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E165" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F165" s="4"/>
+    <row r="165" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E165" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F165" s="3"/>
     </row>
-    <row r="166" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E166" t="s">
         <v>6</v>
       </c>
@@ -15402,7 +15516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E167" s="1" t="s">
         <v>10</v>
       </c>
@@ -15425,7 +15539,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="168" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E168" s="2" t="s">
         <v>12</v>
       </c>
@@ -15440,7 +15554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E169" s="1" t="s">
         <v>11</v>
       </c>
@@ -15463,7 +15577,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="170" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E170" s="2" t="s">
         <v>13</v>
       </c>
@@ -15478,13 +15592,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E186" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F186" s="4"/>
+    <row r="186" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E186" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F186" s="3"/>
     </row>
-    <row r="187" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E187" t="s">
         <v>6</v>
       </c>
@@ -15507,7 +15621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E188" s="1" t="s">
         <v>10</v>
       </c>
@@ -15530,7 +15644,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="189" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E189" s="2" t="s">
         <v>12</v>
       </c>
@@ -15545,7 +15659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E190" s="1" t="s">
         <v>11</v>
       </c>
@@ -15568,7 +15682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="191" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E191" s="2" t="s">
         <v>13</v>
       </c>
@@ -15583,13 +15697,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E201" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F201" s="4"/>
+    <row r="201" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E201" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F201" s="3"/>
     </row>
-    <row r="202" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E202" t="s">
         <v>6</v>
       </c>
@@ -15612,7 +15726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E203" s="1" t="s">
         <v>10</v>
       </c>
@@ -15635,7 +15749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E204" s="2" t="s">
         <v>12</v>
       </c>
@@ -15650,7 +15764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E205" s="1" t="s">
         <v>11</v>
       </c>
@@ -15673,7 +15787,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E206" s="2" t="s">
         <v>13</v>
       </c>
@@ -15709,12 +15823,12 @@
       <selection sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -15737,7 +15851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -15760,7 +15874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -15775,7 +15889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -15798,7 +15912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
all crop types added
</commit_message>
<xml_diff>
--- a/Elixir Crop & Soil Information/SoilTables.xlsx
+++ b/Elixir Crop & Soil Information/SoilTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berkozdoruk/Desktop/GitHub/Elixir-Documentation/Elixir Crop &amp; Soil Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC06AC64-E78B-1E44-AFD2-3EFCCD6A66FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D623B47A-85EC-754F-90F8-1E33790EA76E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9426C972-A351-456A-ACBE-3D80CCCA88B5}"/>
   </bookViews>
@@ -76,18 +76,6 @@
     <t>http://soilquality.org.au/factsheets/water-availability</t>
   </si>
   <si>
-    <t>Table 7</t>
-  </si>
-  <si>
-    <t>Table 8</t>
-  </si>
-  <si>
-    <t>Table 9</t>
-  </si>
-  <si>
-    <t>Table 10</t>
-  </si>
-  <si>
     <t>domates</t>
   </si>
   <si>
@@ -113,6 +101,18 @@
   </si>
   <si>
     <t>Marul</t>
+  </si>
+  <si>
+    <t>Havuc</t>
+  </si>
+  <si>
+    <t>Patlican</t>
+  </si>
+  <si>
+    <t>Kavun</t>
+  </si>
+  <si>
+    <t>Fasulye</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1055,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 9</c:v>
+              <c:v>Kavun</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1305,22 +1305,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,22 +1387,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1703,7 +1703,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 10</c:v>
+              <c:v>Fasulye</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1953,22 +1953,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,22 +2035,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6231,7 +6231,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 7</c:v>
+              <c:v>Havuc</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -6484,19 +6484,19 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6563,22 +6563,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6879,7 +6879,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Table 8</c:v>
+              <c:v>Patlican</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -7129,22 +7129,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7211,22 +7211,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14535,8 +14535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD730A-B317-4AF4-A2AA-E14D92B6C330}">
   <dimension ref="C2:AB206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H156" sqref="H156"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I216" sqref="I216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14668,7 +14668,7 @@
     </row>
     <row r="28" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E28" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -14781,7 +14781,7 @@
     </row>
     <row r="46" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E46" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -14896,7 +14896,7 @@
     </row>
     <row r="62" spans="5:28" x14ac:dyDescent="0.2">
       <c r="Y62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="Z62">
         <v>60</v>
@@ -14907,7 +14907,7 @@
     </row>
     <row r="64" spans="5:28" x14ac:dyDescent="0.2">
       <c r="Y64" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Z64" s="6">
         <v>1</v>
@@ -14934,7 +14934,7 @@
     </row>
     <row r="67" spans="5:28" x14ac:dyDescent="0.2">
       <c r="E67" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F67" s="3"/>
     </row>
@@ -14961,7 +14961,7 @@
         <v>5</v>
       </c>
       <c r="Y68" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="5:28" x14ac:dyDescent="0.2">
@@ -15069,7 +15069,7 @@
     </row>
     <row r="89" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E89" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F89" s="3"/>
     </row>
@@ -15174,7 +15174,7 @@
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E107" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F107" s="3"/>
     </row>
@@ -15279,7 +15279,7 @@
     </row>
     <row r="127" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E127" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F127" s="3"/>
     </row>
@@ -15384,7 +15384,7 @@
     </row>
     <row r="147" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E147" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F147" s="3"/>
     </row>
@@ -15419,19 +15419,19 @@
         <v>5</v>
       </c>
       <c r="G149" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H149" s="1">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I149" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J149" s="1">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K149" s="1">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="5:11" x14ac:dyDescent="0.2">
@@ -15454,22 +15454,22 @@
         <v>11</v>
       </c>
       <c r="F151" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G151" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H151" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I151" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J151" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K151" s="1">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="152" spans="5:11" x14ac:dyDescent="0.2">
@@ -15489,7 +15489,7 @@
     </row>
     <row r="165" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E165" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F165" s="3"/>
     </row>
@@ -15521,22 +15521,22 @@
         <v>10</v>
       </c>
       <c r="F167" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G167" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H167" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I167" s="1">
+        <v>19</v>
+      </c>
+      <c r="J167" s="1">
         <v>24</v>
       </c>
-      <c r="J167" s="1">
+      <c r="K167" s="1">
         <v>28</v>
-      </c>
-      <c r="K167" s="1">
-        <v>546</v>
       </c>
     </row>
     <row r="168" spans="5:11" x14ac:dyDescent="0.2">
@@ -15559,22 +15559,22 @@
         <v>11</v>
       </c>
       <c r="F169" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G169" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H169" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I169" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J169" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K169" s="1">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="5:11" x14ac:dyDescent="0.2">
@@ -15594,7 +15594,7 @@
     </row>
     <row r="186" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E186" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F186" s="3"/>
     </row>
@@ -15626,22 +15626,22 @@
         <v>10</v>
       </c>
       <c r="F188" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G188" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H188" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I188" s="1">
+        <v>19</v>
+      </c>
+      <c r="J188" s="1">
         <v>24</v>
       </c>
-      <c r="J188" s="1">
+      <c r="K188" s="1">
         <v>28</v>
-      </c>
-      <c r="K188" s="1">
-        <v>89</v>
       </c>
     </row>
     <row r="189" spans="5:11" x14ac:dyDescent="0.2">
@@ -15664,22 +15664,22 @@
         <v>11</v>
       </c>
       <c r="F190" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G190" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H190" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I190" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J190" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K190" s="1">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="191" spans="5:11" x14ac:dyDescent="0.2">
@@ -15699,7 +15699,7 @@
     </row>
     <row r="201" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E201" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F201" s="3"/>
     </row>
@@ -15731,22 +15731,22 @@
         <v>10</v>
       </c>
       <c r="F203" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G203" s="1">
+        <v>9</v>
+      </c>
+      <c r="H203" s="1">
         <v>12</v>
       </c>
-      <c r="H203" s="1">
+      <c r="I203" s="1">
+        <v>15</v>
+      </c>
+      <c r="J203" s="1">
         <v>18</v>
       </c>
-      <c r="I203" s="1">
-        <v>24</v>
-      </c>
-      <c r="J203" s="1">
-        <v>28</v>
-      </c>
       <c r="K203" s="1">
-        <v>60</v>
+        <v>22</v>
       </c>
     </row>
     <row r="204" spans="5:11" x14ac:dyDescent="0.2">
@@ -15769,22 +15769,22 @@
         <v>11</v>
       </c>
       <c r="F205" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G205" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H205" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I205" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J205" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="K205" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="206" spans="5:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update crops graphs v2
</commit_message>
<xml_diff>
--- a/Elixir Crop & Soil Information/SoilTables.xlsx
+++ b/Elixir Crop & Soil Information/SoilTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berkozdoruk/Desktop/GitHub/Elixir-Documentation/Elixir Crop &amp; Soil Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053D28D-E83C-E54E-B9A8-393CA373F499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D312CEFF-CF6D-E448-8F8B-645A5600B5A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{9426C972-A351-456A-ACBE-3D80CCCA88B5}"/>
   </bookViews>
@@ -1387,22 +1387,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2044,13 +2044,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2683,22 +2683,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3331,22 +3331,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5191,16 +5191,16 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5267,22 +5267,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>14</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5915,22 +5915,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6563,22 +6563,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7211,22 +7211,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14535,8 +14535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD730A-B317-4AF4-A2AA-E14D92B6C330}">
   <dimension ref="C2:AB206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J214" sqref="J214"/>
+    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I213" sqref="I213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14743,22 +14743,22 @@
         <v>11</v>
       </c>
       <c r="F32" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G32" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H32" s="1">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1">
         <v>12</v>
       </c>
-      <c r="I32" s="1">
-        <v>16</v>
-      </c>
       <c r="J32" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K32" s="1">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="5:23" x14ac:dyDescent="0.2">
@@ -14857,22 +14857,22 @@
         <v>11</v>
       </c>
       <c r="F50" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G50" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H50" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I50" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J50" s="1">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="K50" s="1">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="5:28" x14ac:dyDescent="0.2">
@@ -15212,16 +15212,16 @@
         <v>9</v>
       </c>
       <c r="H109" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I109" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J109" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K109" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="5:11" x14ac:dyDescent="0.2">
@@ -15244,22 +15244,22 @@
         <v>11</v>
       </c>
       <c r="F111" s="1">
+        <v>2</v>
+      </c>
+      <c r="G111" s="1">
         <v>4</v>
       </c>
-      <c r="G111" s="1">
+      <c r="H111" s="1">
         <v>7</v>
       </c>
-      <c r="H111" s="1">
+      <c r="I111" s="1">
         <v>10</v>
       </c>
-      <c r="I111" s="1">
-        <v>14</v>
-      </c>
       <c r="J111" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K111" s="1">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="5:11" x14ac:dyDescent="0.2">
@@ -15349,22 +15349,22 @@
         <v>11</v>
       </c>
       <c r="F131" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G131" s="1">
+        <v>4</v>
+      </c>
+      <c r="H131" s="1">
+        <v>8</v>
+      </c>
+      <c r="I131" s="1">
         <v>10</v>
       </c>
-      <c r="H131" s="1">
-        <v>14</v>
-      </c>
-      <c r="I131" s="1">
-        <v>19</v>
-      </c>
       <c r="J131" s="1">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K131" s="1">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="5:11" x14ac:dyDescent="0.2">
@@ -15454,22 +15454,22 @@
         <v>11</v>
       </c>
       <c r="F151" s="1">
+        <v>1</v>
+      </c>
+      <c r="G151" s="1">
+        <v>2</v>
+      </c>
+      <c r="H151" s="1">
         <v>4</v>
       </c>
-      <c r="G151" s="1">
+      <c r="I151" s="1">
         <v>6</v>
       </c>
-      <c r="H151" s="1">
+      <c r="J151" s="1">
         <v>9</v>
       </c>
-      <c r="I151" s="1">
+      <c r="K151" s="1">
         <v>12</v>
-      </c>
-      <c r="J151" s="1">
-        <v>15</v>
-      </c>
-      <c r="K151" s="1">
-        <v>18</v>
       </c>
     </row>
     <row r="152" spans="5:11" x14ac:dyDescent="0.2">
@@ -15559,22 +15559,22 @@
         <v>11</v>
       </c>
       <c r="F169" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G169" s="1">
         <v>7</v>
       </c>
       <c r="H169" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I169" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J169" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K169" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="170" spans="5:11" x14ac:dyDescent="0.2">
@@ -15664,22 +15664,22 @@
         <v>11</v>
       </c>
       <c r="F190" s="1">
+        <v>1</v>
+      </c>
+      <c r="G190" s="1">
+        <v>2</v>
+      </c>
+      <c r="H190" s="1">
         <v>4</v>
       </c>
-      <c r="G190" s="1">
-        <v>7</v>
-      </c>
-      <c r="H190" s="1">
-        <v>10</v>
-      </c>
       <c r="I190" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J190" s="1">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="K190" s="1">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="5:11" x14ac:dyDescent="0.2">
@@ -15778,13 +15778,13 @@
         <v>8</v>
       </c>
       <c r="I205" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J205" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K205" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="5:11" x14ac:dyDescent="0.2">

</xml_diff>